<commit_message>
Use spintax to send email body
</commit_message>
<xml_diff>
--- a/Email_Data.xlsx
+++ b/Email_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenpohsuan/Desktop/Social Media Ministries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenpohsuan/Desktop/Social Media Ministries/Auto_Send_Email_Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416C11B4-E351-BF4D-B4C8-ECAE41C00A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB24586D-92B0-DC4D-AE40-13D92C6A5B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="4660" windowWidth="12220" windowHeight="7660" activeTab="1" xr2:uid="{B34CFBD0-74FD-2D48-BBA1-8F27113A7D6D}"/>
+    <workbookView xWindow="9660" yWindow="4660" windowWidth="12220" windowHeight="7660" xr2:uid="{B34CFBD0-74FD-2D48-BBA1-8F27113A7D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Receiver Info" sheetId="1" r:id="rId1"/>
@@ -36,25 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>Email Subject</t>
-  </si>
-  <si>
-    <t>Email body</t>
-  </si>
-  <si>
-    <t>[Test Email]-2</t>
-  </si>
-  <si>
-    <t>[Test Email]-1</t>
-  </si>
-  <si>
-    <t>Hi! This is a test email-1.</t>
-  </si>
-  <si>
-    <t>Hi! This is a test email-2.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Sender Email</t>
   </si>
@@ -429,50 +411,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C6F63F-BE0C-8347-8D05-11C0C36F0C13}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -484,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE3EAF1-29EC-6E4A-9270-A49A51BB9FDE}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,18 +458,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>